<commit_message>
new task list in xlsx
</commit_message>
<xml_diff>
--- a/task_list/NewTaskList.xlsx
+++ b/task_list/NewTaskList.xlsx
@@ -2670,41 +2670,41 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B30:F30"/>
     <mergeCell ref="C3:F3"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B39:F39"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
modified excel for nice pdf exporting and aded pdf
</commit_message>
<xml_diff>
--- a/task_list/NewTaskList.xlsx
+++ b/task_list/NewTaskList.xlsx
@@ -1,24 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Carlos/Desktop/nyu_cs_classes/rbda/project/crime/task_list/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="20480"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$E$46</definedName>
+  </definedNames>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>Big Data Analytics Project Task List</t>
   </si>
   <si>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="14"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -80,7 +99,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -106,7 +125,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -129,7 +148,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -140,7 +159,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -151,7 +170,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -162,7 +181,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -248,7 +267,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -262,7 +281,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -279,7 +298,7 @@
   <si>
     <r>
       <rPr>
-        <i val="1"/>
+        <i/>
         <sz val="12"/>
         <color indexed="8"/>
         <rFont val="Arial"/>
@@ -297,28 +316,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="18"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -329,13 +335,13 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <i val="1"/>
+      <i/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -346,23 +352,27 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
-      <i val="1"/>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
-      <i val="1"/>
+      <i/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -397,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -630,19 +640,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -663,30 +660,6 @@
       </top>
       <bottom style="thin">
         <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -718,15 +691,6 @@
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -771,214 +735,240 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="53">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="15" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="9" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff92cddc"/>
-      <rgbColor rgb="ffdaeef3"/>
-      <rgbColor rgb="fffde9d9"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF92CDDC"/>
+      <rgbColor rgb="FFDAEEF3"/>
+      <rgbColor rgb="FFFDE9D9"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -1104,7 +1094,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1113,7 +1103,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1122,7 +1112,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1196,7 +1186,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1204,7 +1194,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1223,7 +1213,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1243,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1269,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1295,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1321,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1357,7 +1347,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,7 +1373,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1409,7 +1399,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1435,7 +1425,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1461,7 +1451,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1474,9 +1464,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1491,7 +1487,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -1499,7 +1495,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1518,7 +1514,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1544,7 +1540,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1570,7 +1566,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1596,7 +1592,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1622,7 +1618,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1648,7 +1644,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1674,7 +1670,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1700,7 +1696,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1726,7 +1722,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1752,7 +1748,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1765,9 +1761,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1781,7 +1783,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1800,7 +1802,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1830,7 +1832,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1856,7 +1858,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1882,7 +1884,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1908,7 +1910,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1934,7 +1936,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1960,7 +1962,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1986,7 +1988,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2012,7 +2014,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2038,7 +2040,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2051,665 +2053,638 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.17188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.3516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.8516" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="58.6719" style="1" customWidth="1"/>
-    <col min="7" max="256" width="12.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="58.6640625" style="1" customWidth="1"/>
+    <col min="6" max="255" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="81.1" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+    <row r="1" spans="1:5" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
-    </row>
-    <row r="2" ht="45" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s" s="6">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" ht="33" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" t="s" s="10">
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+    </row>
+    <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s" s="11">
+      <c r="B3" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" ht="30" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="14"/>
-      <c r="C4" t="s" s="15">
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="35"/>
+      <c r="B4" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" ht="30" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="18"/>
-      <c r="C5" t="s" s="15">
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36"/>
+      <c r="B5" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" ht="8" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" ht="28" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" t="s" s="24">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="49"/>
+    </row>
+    <row r="6" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
+    </row>
+    <row r="7" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s" s="24">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s" s="24">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s" s="24">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" t="s" s="24">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="8" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-    </row>
-    <row r="9" ht="26" customHeight="1">
-      <c r="A9" s="27"/>
-      <c r="B9" t="s" s="28">
+    <row r="8" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+    </row>
+    <row r="9" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
-    </row>
-    <row r="10" ht="31" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" t="s" s="31">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s" s="32">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s" s="33">
+      <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E10" t="s" s="33">
+      <c r="D10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" ht="30" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" t="s" s="31">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s" s="32">
+      <c r="B11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s" s="33">
+      <c r="C11" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="s" s="35">
+      <c r="D11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F11" t="s" s="36">
+      <c r="E11" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" ht="45" customHeight="1">
+    <row r="12" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="40"/>
-      <c r="F12" t="s" s="41">
+      <c r="B12" s="24"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" ht="8" customHeight="1">
-      <c r="A13" s="23"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-    </row>
-    <row r="14" ht="26" customHeight="1">
-      <c r="A14" s="27"/>
-      <c r="B14" t="s" s="28">
+    <row r="13" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="41"/>
+    </row>
+    <row r="14" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-    </row>
-    <row r="15" ht="36" customHeight="1">
-      <c r="A15" s="2"/>
-      <c r="B15" t="s" s="31">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s" s="33">
+      <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D15" t="s" s="33">
+      <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E15" t="s" s="33">
+      <c r="D15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F15" t="s" s="42">
+      <c r="E15" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" ht="34" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" t="s" s="31">
+    <row r="16" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C16" t="s" s="43">
+      <c r="B16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s" s="43">
+      <c r="C16" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E16" t="s" s="43">
+      <c r="D16" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F16" t="s" s="36">
+      <c r="E16" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" ht="60" customHeight="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" t="s" s="45">
+    <row r="17" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" ht="27" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" t="s" s="45">
+    <row r="18" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" ht="22" customHeight="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" t="s" s="41">
+    <row r="19" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="19"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" ht="35" customHeight="1">
-      <c r="A20" s="19"/>
-      <c r="B20" t="s" s="31">
+    <row r="20" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C20" t="s" s="33">
+      <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s" s="33">
+      <c r="C20" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E20" t="s" s="33">
+      <c r="D20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="34"/>
-    </row>
-    <row r="21" ht="8" customHeight="1">
-      <c r="A21" s="23"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" ht="26" customHeight="1">
-      <c r="A22" s="27"/>
-      <c r="B22" t="s" s="28">
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="39"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="41"/>
+    </row>
+    <row r="22" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
-    </row>
-    <row r="23" ht="36" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" t="s" s="31">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C23" t="s" s="33">
+      <c r="B23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D23" t="s" s="33">
+      <c r="C23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E23" t="s" s="33">
+      <c r="D23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F23" t="s" s="42">
+      <c r="E23" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" ht="34" customHeight="1">
-      <c r="A24" s="2"/>
-      <c r="B24" t="s" s="31">
+    <row r="24" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C24" t="s" s="43">
+      <c r="B24" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D24" t="s" s="43">
+      <c r="C24" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E24" t="s" s="43">
+      <c r="D24" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F24" t="s" s="36">
+      <c r="E24" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" ht="60" customHeight="1">
-      <c r="A25" s="2"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" t="s" s="45">
+    <row r="25" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="19"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="2"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
-      <c r="F26" t="s" s="45">
+    <row r="26" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="19"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" ht="22" customHeight="1">
-      <c r="A27" s="2"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" t="s" s="41">
+    <row r="27" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="19"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" ht="35" customHeight="1">
-      <c r="A28" s="19"/>
-      <c r="B28" t="s" s="31">
+    <row r="28" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C28" t="s" s="33">
+      <c r="B28" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D28" t="s" s="33">
+      <c r="C28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E28" t="s" s="33">
+      <c r="D28" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="34"/>
-    </row>
-    <row r="29" ht="8" customHeight="1">
-      <c r="A29" s="23"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="26"/>
-    </row>
-    <row r="30" ht="26" customHeight="1">
-      <c r="A30" s="27"/>
-      <c r="B30" t="s" s="28">
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="41"/>
+    </row>
+    <row r="30" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30"/>
-    </row>
-    <row r="31" ht="36" customHeight="1">
-      <c r="A31" s="2"/>
-      <c r="B31" t="s" s="31">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C31" t="s" s="33">
+      <c r="B31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D31" t="s" s="33">
+      <c r="C31" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E31" t="s" s="33">
+      <c r="D31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F31" t="s" s="42">
+      <c r="E31" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" ht="34" customHeight="1">
-      <c r="A32" s="2"/>
-      <c r="B32" t="s" s="31">
+    <row r="32" spans="1:5" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C32" t="s" s="43">
+      <c r="B32" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D32" t="s" s="43">
+      <c r="C32" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E32" t="s" s="43">
+      <c r="D32" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F32" t="s" s="36">
+      <c r="E32" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" ht="60" customHeight="1">
-      <c r="A33" s="2"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="44"/>
-      <c r="F33" t="s" s="45">
+    <row r="33" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="19"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" ht="27" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="44"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" t="s" s="45">
+    <row r="34" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="19"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" ht="22" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" t="s" s="41">
+    <row r="35" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="19"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" ht="35" customHeight="1">
-      <c r="A36" s="19"/>
-      <c r="B36" t="s" s="31">
+    <row r="36" spans="1:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C36" t="s" s="33">
+      <c r="B36" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D36" t="s" s="33">
+      <c r="C36" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E36" t="s" s="33">
+      <c r="D36" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F36" s="34"/>
-    </row>
-    <row r="37" ht="8" customHeight="1">
-      <c r="A37" s="47"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="49"/>
-    </row>
-    <row r="38" ht="26" customHeight="1">
-      <c r="A38" s="47"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="51"/>
-    </row>
-    <row r="39" ht="36" customHeight="1">
-      <c r="A39" s="52"/>
-      <c r="B39" t="s" s="28">
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="38"/>
+    </row>
+    <row r="38" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="26"/>
+    </row>
+    <row r="39" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="30"/>
-    </row>
-    <row r="40" ht="35.2" customHeight="1">
-      <c r="A40" s="52"/>
-      <c r="B40" t="s" s="31">
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="17"/>
+    </row>
+    <row r="40" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C40" t="s" s="32">
+      <c r="B40" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D40" t="s" s="33">
+      <c r="C40" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E40" t="s" s="33">
+      <c r="D40" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F40" t="s" s="53">
+      <c r="E40" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" ht="35.85" customHeight="1">
-      <c r="A41" s="52"/>
-      <c r="B41" t="s" s="31">
+    <row r="41" spans="1:5" ht="35.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C41" t="s" s="32">
+      <c r="B41" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D41" t="s" s="33">
+      <c r="C41" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E41" t="s" s="33">
+      <c r="D41" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F41" t="s" s="53">
+      <c r="E41" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" ht="34.8" customHeight="1">
-      <c r="A42" s="52"/>
-      <c r="B42" t="s" s="31">
+    <row r="42" spans="1:5" ht="34.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C42" t="s" s="32">
+      <c r="B42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D42" t="s" s="33">
+      <c r="C42" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E42" t="s" s="33">
+      <c r="D42" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F42" t="s" s="53">
+      <c r="E42" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" ht="30.4" customHeight="1">
-      <c r="A43" s="27"/>
-      <c r="B43" t="s" s="31">
+    <row r="43" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C43" t="s" s="32">
+      <c r="B43" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D43" t="s" s="33">
+      <c r="C43" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E43" t="s" s="33">
+      <c r="D43" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F43" t="s" s="36">
+      <c r="E43" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" ht="30.25" customHeight="1">
-      <c r="A44" s="2"/>
-      <c r="B44" s="37"/>
-      <c r="C44" t="s" s="32">
+    <row r="44" spans="1:5" ht="30.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="19"/>
+      <c r="B44" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D44" t="s" s="33">
+      <c r="C44" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E44" t="s" s="33">
+      <c r="D44" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F44" t="s" s="41">
+      <c r="E44" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" ht="30.6" customHeight="1">
-      <c r="A45" s="54"/>
-      <c r="B45" t="s" s="31">
+    <row r="45" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C45" t="s" s="32">
+      <c r="B45" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D45" t="s" s="33">
+      <c r="C45" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E45" t="s" s="33">
+      <c r="D45" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F45" t="s" s="42">
+      <c r="E45" s="10" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="46" ht="30.4" customHeight="1">
-      <c r="A46" s="55"/>
-      <c r="B46" t="s" s="31">
+    <row r="46" spans="1:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C46" t="s" s="32">
+      <c r="B46" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D46" t="s" s="56">
+      <c r="C46" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="57">
+      <c r="D46" s="14">
         <v>43084</v>
       </c>
-      <c r="F46" s="34"/>
+      <c r="E46" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A43:A44"/>
     <mergeCell ref="B16:B19"/>
-    <mergeCell ref="D32:D35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="D24:D27"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A16:A19"/>
     <mergeCell ref="C32:C35"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="A32:A35"/>
     <mergeCell ref="C24:C27"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="C3:F3"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup scale="46" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="46" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="5" max="1048575" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
</xml_diff>